<commit_message>
create final Rmd for Ohio
</commit_message>
<xml_diff>
--- a/data/ohio/stops.xlsx
+++ b/data/ohio/stops.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\herşey\R_projects\GTFS_for_Athens\data\ohio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B699D9C-CB7E-457F-98F1-D4E98DD48061}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A02BA76-F00E-432F-984C-32B1075F5B1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13460" yWindow="1850" windowWidth="10710" windowHeight="8440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -653,661 +653,775 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>41.068637000000003</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>-81.524315000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>39.234185444432299</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>-82.196805583952994</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>39.337581083333298</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>-82.075599520833293</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>39.324967654976902</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>-82.102466735083595</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>39.082903195262602</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>-84.152953196812703</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>15</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>41.3157898077325</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>-81.653323942789996</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>17</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>39.738387766040603</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>-81.530170801648495</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>19</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>39.991393404109601</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>-81.573141732876707</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>21</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>40.797874387755101</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>-81.370974693877599</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
         <v>22</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>23</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>39.113182724413399</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>-84.500097832195195</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>24</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>25</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>39.133891823575702</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>-84.509238295836198</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>26</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>27</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>41.5031872828283</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>-81.682033767676799</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
         <v>28</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>29</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>40.811192539898897</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>-81.929473003468701</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
         <v>30</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>31</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>39.998531472535497</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>-82.892500652061202</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
         <v>32</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>33</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>39.959094069335997</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>-82.996793286879395</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>34</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>35</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>39.222244763663198</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>-81.809730001849005</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
         <v>36</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>37</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>40.846863530515598</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>-84.319138781744797</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
         <v>38</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>39</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>40.378328150000002</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>-82.396253238445098</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>40</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>41</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>40.3686048379585</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>-82.397225883497001</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
         <v>42</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>43</v>
       </c>
-      <c r="C21">
+      <c r="D21">
         <v>39.037348049999999</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>-82.624113794364305</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
         <v>44</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>45</v>
       </c>
-      <c r="C22">
+      <c r="D22">
         <v>40.6454570816326</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>-83.608171428571396</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B23" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="1">
+      <c r="D23" s="1">
         <v>34.493132299999999</v>
       </c>
-      <c r="D23" s="1">
+      <c r="E23" s="1">
         <v>136.69040050000001</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
         <v>48</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>49</v>
       </c>
-      <c r="C24">
+      <c r="D24">
         <v>40.741280183673503</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>-84.1028825510204</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
         <v>50</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>51</v>
       </c>
-      <c r="C25">
+      <c r="D25">
         <v>39.517045000000003</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>-82.363780000000006</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
         <v>52</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>53</v>
       </c>
-      <c r="C26">
+      <c r="D26">
         <v>40.601660448962697</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>-82.263047394180802</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
         <v>54</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>55</v>
       </c>
-      <c r="C27">
+      <c r="D27">
         <v>40.756330900000002</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <v>-82.5144769864757</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
         <v>56</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>57</v>
       </c>
-      <c r="C28">
+      <c r="D28">
         <v>39.413155199999999</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>-81.455303299999997</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
         <v>58</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>59</v>
       </c>
-      <c r="C29">
+      <c r="D29">
         <v>40.270700968140098</v>
       </c>
-      <c r="D29">
+      <c r="E29">
         <v>-82.359661945218406</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
         <v>60</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>61</v>
       </c>
-      <c r="C30">
+      <c r="D30">
         <v>40.240635766461999</v>
       </c>
-      <c r="D30">
+      <c r="E30">
         <v>-83.3417422028906</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
         <v>62</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>63</v>
       </c>
-      <c r="C31">
+      <c r="D31">
         <v>40.693141300000001</v>
       </c>
-      <c r="D31">
+      <c r="E31">
         <v>-81.698767799999999</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
         <v>64</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>65</v>
       </c>
-      <c r="C32">
+      <c r="D32">
         <v>40.494810749999999</v>
       </c>
-      <c r="D32">
+      <c r="E32">
         <v>-82.714950965771905</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
         <v>66</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>67</v>
       </c>
-      <c r="C33">
+      <c r="D33">
         <v>40.384574959183702</v>
       </c>
-      <c r="D33">
+      <c r="E33">
         <v>-82.481853428571398</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
         <v>68</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>69</v>
       </c>
-      <c r="C34">
+      <c r="D34">
         <v>39.442182000000003</v>
       </c>
-      <c r="D34">
+      <c r="E34">
         <v>-82.222088999999997</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
         <v>70</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>71</v>
       </c>
-      <c r="C35">
+      <c r="D35">
         <v>40.491876901847697</v>
       </c>
-      <c r="D35">
+      <c r="E35">
         <v>-81.481297102880305</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
         <v>72</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>73</v>
       </c>
-      <c r="C36">
+      <c r="D36">
         <v>40.070770470178999</v>
       </c>
-      <c r="D36">
+      <c r="E36">
         <v>-82.444958256266304</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
         <v>74</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>75</v>
       </c>
-      <c r="C37">
+      <c r="D37">
         <v>40.286569639839101</v>
       </c>
-      <c r="D37">
+      <c r="E37">
         <v>-81.564200806323498</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
         <v>76</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>77</v>
       </c>
-      <c r="C38">
+      <c r="D38">
         <v>39.228019119087698</v>
       </c>
-      <c r="D38">
+      <c r="E38">
         <v>-81.516891756708802</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
         <v>78</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>79</v>
       </c>
-      <c r="C39">
+      <c r="D39">
         <v>41.418816629119199</v>
       </c>
-      <c r="D39">
+      <c r="E39">
         <v>-81.781645501478806</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
         <v>80</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>81</v>
       </c>
-      <c r="C40">
+      <c r="D40">
         <v>38.932899432604501</v>
       </c>
-      <c r="D40">
+      <c r="E40">
         <v>-83.417927516437004</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
         <v>82</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>83</v>
       </c>
-      <c r="C41">
+      <c r="D41">
         <v>39.0626082</v>
       </c>
-      <c r="D41">
+      <c r="E41">
         <v>-83.017178900000005</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
         <v>84</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>85</v>
       </c>
-      <c r="C42">
+      <c r="D42">
         <v>39.034428506152899</v>
       </c>
-      <c r="D42">
+      <c r="E42">
         <v>-83.563848894437101</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
         <v>86</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>87</v>
       </c>
-      <c r="C43">
+      <c r="D43">
         <v>40.680351421052599</v>
       </c>
-      <c r="D43">
+      <c r="E43">
         <v>-82.024874192982494</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
         <v>88</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>89</v>
       </c>
-      <c r="C44">
+      <c r="D44">
         <v>40.874099695310903</v>
       </c>
-      <c r="D44">
+      <c r="E44">
         <v>-84.599955747479797</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
         <v>90</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>91</v>
       </c>
-      <c r="C45">
+      <c r="D45">
         <v>41.662455749999999</v>
       </c>
-      <c r="D45">
+      <c r="E45">
         <v>-86.129695499999997</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
         <v>92</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>93</v>
       </c>
-      <c r="C46">
+      <c r="D46">
         <v>40.828320499999997</v>
       </c>
-      <c r="D46">
+      <c r="E46">
         <v>-81.909918500000003</v>
       </c>
     </row>
@@ -1321,8 +1435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAD45F7D-9E4F-49CE-ABD5-12C8732A8EC9}">
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>